<commit_message>
Correcion documentacion y mockaups
Correcion
</commit_message>
<xml_diff>
--- a/Documentacion/Product_Backlog.xlsx
+++ b/Documentacion/Product_Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPOCH\8.OCTAVO\Apli2\Repositorio\SistemaBoletosBus\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C0B38-CD41-4B96-92EE-244E25B9B735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC1A12-CA74-49E4-9133-507F3F95D120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Product_Backlog" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Product_Backlog!$A$1:$I$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Product_Backlog!$A$1:$I$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="149">
   <si>
     <t>Identificador (ID) de la Historia</t>
   </si>
@@ -216,12 +216,6 @@
     <t>HT-09</t>
   </si>
   <si>
-    <t>Implementación de pasarela de pagos</t>
-  </si>
-  <si>
-    <t>Pasarela de pagos</t>
-  </si>
-  <si>
     <t>Servidor base de datos</t>
   </si>
   <si>
@@ -469,6 +463,27 @@
   </si>
   <si>
     <t>Actualización estado Sprint 3</t>
+  </si>
+  <si>
+    <t>Implementación de metodo de pago alternativo</t>
+  </si>
+  <si>
+    <t>Metodo de pago</t>
+  </si>
+  <si>
+    <t>Maquetado de interfaces</t>
+  </si>
+  <si>
+    <t>HT-14</t>
+  </si>
+  <si>
+    <t>Detalle en HT-14</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Actualización Product Backlog</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1072,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,7 +1147,7 @@
     <row r="6" spans="1:10" ht="32.85" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1146,19 +1161,19 @@
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="E7" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="F7" s="21" t="s">
         <v>131</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>133</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1171,16 +1186,16 @@
         <v>45252</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D8" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>137</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>139</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1193,16 +1208,16 @@
         <v>45255</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1215,16 +1230,16 @@
         <v>45265</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1237,29 +1252,39 @@
         <v>45270</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="25.95" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="B12" s="18">
+        <v>45307</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>148</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1394,10 +1419,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1417,12 +1442,12 @@
   <sheetData>
     <row r="1" spans="2:9" ht="36.299999999999997" x14ac:dyDescent="0.7">
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="21.35" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1462,13 +1487,13 @@
         <v>52</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>10</v>
@@ -1488,13 +1513,13 @@
         <v>53</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>10</v>
@@ -1508,19 +1533,19 @@
         <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>10</v>
@@ -1534,19 +1559,19 @@
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>10</v>
@@ -1566,13 +1591,13 @@
         <v>55</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>10</v>
@@ -1583,80 +1608,80 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
@@ -1670,13 +1695,13 @@
         <v>56</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>10</v>
@@ -1687,54 +1712,54 @@
     </row>
     <row r="14" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1748,13 +1773,13 @@
         <v>33</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>10</v>
@@ -1763,7 +1788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
@@ -1774,16 +1799,16 @@
         <v>34</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>32</v>
@@ -1800,13 +1825,13 @@
         <v>43</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>10</v>
@@ -1826,13 +1851,13 @@
         <v>42</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>44</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>10</v>
@@ -1852,13 +1877,13 @@
         <v>46</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>48</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>10</v>
@@ -1872,155 +1897,181 @@
         <v>58</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>101</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="13" t="s">
-        <v>84</v>
+      <c r="B23" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" s="5" t="s">
+      <c r="D27" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="16" t="s">
+      <c r="F27" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>